<commit_message>
Added updated code for Children & Adolescents Dataset
</commit_message>
<xml_diff>
--- a/Autism_Child_data_in_excel.xlsx
+++ b/Autism_Child_data_in_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\STUDY\Projects\Autism-Child\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897AAC5B-9CF2-4A5F-B3D6-CDEC991B64C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403DECC5-2441-4EED-82C5-FC32E579EBCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7EB5FFAB-6DF7-4059-A378-FB1858B4E81D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{7EB5FFAB-6DF7-4059-A378-FB1858B4E81D}"/>
   </bookViews>
   <sheets>
     <sheet name="Autism_Child" sheetId="1" r:id="rId1"/>
@@ -846,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC49043-E442-404B-B57B-388F8CD9307F}">
   <dimension ref="A1:U293"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A266" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -19923,9 +19923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EABB84-6C98-46A1-905C-E84A7985C187}">
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>